<commit_message>
added registration form using payload format
</commit_message>
<xml_diff>
--- a/config/default/forms/app/registration.xlsx
+++ b/config/default/forms/app/registration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Test\Desktop\kpif\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFEA1302-7902-45F8-812D-18F3B3957B48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4C71D1-298E-4F1F-9869-8F99E7917009}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="200">
   <si>
     <t>type</t>
   </si>
@@ -629,6 +629,12 @@
   </si>
   <si>
     <t>patient_passportNumber</t>
+  </si>
+  <si>
+    <t>registration</t>
+  </si>
+  <si>
+    <t>Registration</t>
   </si>
 </sst>
 </file>
@@ -4045,7 +4051,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -7559,7 +7565,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:6" ht="27">
+    <row r="2" spans="1:6" ht="13.5">
       <c r="A2" s="11" t="s">
         <v>74</v>
       </c>
@@ -7922,9 +7928,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -7956,14 +7962,14 @@
     </row>
     <row r="2" spans="1:6" ht="13.5">
       <c r="A2" s="11" t="s">
-        <v>25</v>
+        <v>199</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>24</v>
+        <v>198</v>
       </c>
       <c r="C2" s="12">
         <f ca="1">NOW()</f>
-        <v>44041.724166550928</v>
+        <v>44041.843359259263</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>62</v>

</xml_diff>